<commit_message>
update camera va thanh gia do cho camera
</commit_message>
<xml_diff>
--- a/6. LINH WORKSPACE/US-11-List-thiet-bi-module-camera.xlsx
+++ b/6. LINH WORKSPACE/US-11-List-thiet-bi-module-camera.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36b6ff3106d558d9/Desktop/robot-vision-system/6. LINH WORKSPACE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E542454F-CBB3-4E4C-A241-DE8FE201254C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{E542454F-CBB3-4E4C-A241-DE8FE201254C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{081FB898-6F86-428F-AB2F-6D1BA90CA90A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{A5CDFF95-7873-4DD0-BB70-D1A5DB9166F4}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="20676" windowHeight="18576" xr2:uid="{A5CDFF95-7873-4DD0-BB70-D1A5DB9166F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Tên hàng / Mục đích sử dụng</t>
   </si>
@@ -117,20 +117,6 @@
     <t>thanh</t>
   </si>
   <si>
-    <t>Thanh INOX / dùng làm thanh đỡ cho hộp camera</t>
-  </si>
-  <si>
-    <t>Xưởng vật dụng mở shop Palia
-Email: paliavietnam@gmail.com</t>
-  </si>
-  <si>
-    <t>Ke chữ L 5X5cm</t>
-  </si>
-  <si>
-    <t>HV Store
-Hotline: 0906236862</t>
-  </si>
-  <si>
     <t xml:space="preserve">Camera 8MP Varifocal </t>
   </si>
   <si>
@@ -138,9 +124,6 @@
   </si>
   <si>
     <t xml:space="preserve">mét </t>
-  </si>
-  <si>
-    <t>TC</t>
   </si>
   <si>
     <t>Giá chưa bao gồm VAT, phí ship</t>
@@ -150,6 +133,37 @@
 Địa chỉ: Tòa nhà GP Invest, 170 Đê La Thành, Ô Chợ Dừa, Đống Đa, Hà Nội
 Hotline: 0763161222
 Email: info@kyoo.info</t>
+  </si>
+  <si>
+    <t>Thanh nhôm định hình 2020 800mm</t>
+  </si>
+  <si>
+    <t>Ke vuông góc cho nhôm định hình chìm 2020</t>
+  </si>
+  <si>
+    <t>Pad chữ L cố định nhôm định hình</t>
+  </si>
+  <si>
+    <t>Cơ khí điện tử
+Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Link kiện cơ khí
+Quận 1, thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Giá chưa bao gồm phí ship</t>
+  </si>
+  <si>
+    <t>Có thể mua tại shop ở Đà Nẵng</t>
+  </si>
+  <si>
+    <t>Thiết bị điện Hàn Quốc
+Long Thành, Đồng Nai
+Số đt: 0938276224 - 0938096421</t>
+  </si>
+  <si>
+    <t>Tấm nhựa Pom/ Dùng để kết nối thanh nhôm với hộp đựng camera</t>
   </si>
 </sst>
 </file>
@@ -222,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,12 +248,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -575,15 +583,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27381B23-575C-44F2-A1BD-FC7801FF8CA2}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
@@ -621,7 +629,7 @@
     </row>
     <row r="2" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -635,14 +643,14 @@
       <c r="E2" s="2">
         <v>3190000</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
@@ -653,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2">
         <v>40000</v>
@@ -661,181 +669,248 @@
       <c r="E3" s="2">
         <v>44000</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>18000</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>36000</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>10000</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>20000</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>5</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="7">
         <v>4000</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>20000</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>25000</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>25000</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>2</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>25000</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>82000</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="9">
-        <v>140000</v>
-      </c>
-      <c r="E9" s="9">
-        <v>172000</v>
+      <c r="D9" s="7">
+        <v>82000</v>
+      </c>
+      <c r="E9" s="7">
+        <v>164000</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>25</v>
+      <c r="G9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="9">
+        <v>30</v>
+      </c>
+      <c r="B10" s="7">
         <v>10</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="9">
-        <v>1300</v>
-      </c>
-      <c r="E10" s="9">
-        <v>13000</v>
+      <c r="D10" s="7">
+        <v>9000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>90000</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C11" s="9"/>
-      <c r="D11" t="s">
+      <c r="G10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7">
+        <v>14000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>56000</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="7">
+        <v>52000</v>
+      </c>
+      <c r="E12" s="7">
+        <v>52000</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -846,11 +921,13 @@
     <hyperlink ref="F6" r:id="rId4" xr:uid="{A911CBB0-C989-4760-AD86-46154BD805B7}"/>
     <hyperlink ref="F7" r:id="rId5" xr:uid="{134B6819-78CE-43B6-AE5F-23FCDFC2698D}"/>
     <hyperlink ref="F8" r:id="rId6" xr:uid="{3F77CBF7-2ECF-4BC8-BB7A-A44D310DD344}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{265EDFD4-ED05-4211-AC5F-A0053EDDB210}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{CB2E1644-CFEF-4AF1-B8C7-EF6496ADB49B}"/>
-    <hyperlink ref="F2" r:id="rId9" xr:uid="{353D54F9-4638-4EAC-AF4F-21C8AE121672}"/>
+    <hyperlink ref="F2" r:id="rId7" xr:uid="{353D54F9-4638-4EAC-AF4F-21C8AE121672}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{4C2AF4A5-2B0E-4A56-AC6D-F1F5E5FB60A6}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{FBEB4707-585B-4E92-A3E6-A3F64403BB0C}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{C6FCB1B6-FBA7-4AE5-80F0-887F3F08009B}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{2CD7F394-6B5D-447D-BB57-9E4D5270EAD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>